<commit_message>
Changes for Dialogflow and Watson full conversation
</commit_message>
<xml_diff>
--- a/testdata/dialogflow/xlsx/Book2.xlsx
+++ b/testdata/dialogflow/xlsx/Book2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>User</t>
   </si>
@@ -67,24 +67,12 @@
     <t>I can help with that. Where would you like to reserve a room?</t>
   </si>
   <si>
-    <t>book room in Florida</t>
-  </si>
-  <si>
-    <t>02/06/2018</t>
-  </si>
-  <si>
     <t>What time will the meeting start?</t>
   </si>
   <si>
-    <t>10 AM</t>
-  </si>
-  <si>
     <t>How long will it last?</t>
   </si>
   <si>
-    <t>1 Hour</t>
-  </si>
-  <si>
     <t>Thanks. How many people are attending?</t>
   </si>
   <si>
@@ -97,7 +85,25 @@
     <t>Hi! I'm your room booking bot. I can help you to find a perfect room for your meeting and manage your reservations.</t>
   </si>
   <si>
-    <t>What is the date?</t>
+    <t>Choose a room please.</t>
+  </si>
+  <si>
+    <t>book a room in Florida</t>
+  </si>
+  <si>
+    <t>02/06/18</t>
+  </si>
+  <si>
+    <t>10:00 AM</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>3 people</t>
+  </si>
+  <si>
+    <t>What date?</t>
   </si>
 </sst>
 </file>
@@ -466,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -508,41 +514,51 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -584,17 +600,17 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>